<commit_message>
modif de la quantité page panier en cours
</commit_message>
<xml_diff>
--- a/DW+P5+-+Modele+plan+tests+acceptation (1).xlsx
+++ b/DW+P5+-+Modele+plan+tests+acceptation (1).xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="588" yWindow="588" windowWidth="21852" windowHeight="8676"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Feuille 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -38,31 +41,83 @@
   </si>
   <si>
     <t>...</t>
+  </si>
+  <si>
+    <t>Une page “produit” qui affiche (de manière dynamique) les détails du produit sur lequel l'utilisateur a cliqué depuis la page d’accueil. Depuis cette page, l’utilisateur peut sélectionner une quantité, une couleur, et ajouter le produit à son panier</t>
+  </si>
+  <si>
+    <t>Une page “confirmation” :
+○ Un message de confirmation de commande, remerciant l'utilisateur pour sa
+commande, et indiquant l'identifiant de commande envoyé par l’API.</t>
+  </si>
+  <si>
+    <t>Ouvrir une page produit avec tout les détails de celui-ci: nom, couleur,quantité que l'utilisateur peut choisir,prix,photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affichage du produit demander </t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Une page “panier”:Un formulaire permettant de passer une commande. Les données du
+formulaire doivent être correctes et bien formatées avant d'être renvoyées au
+back-end. Par exemple, pas de chiffre dans un champ prénom.
+</t>
+  </si>
+  <si>
+    <t>Une page “panier”.  ○ Un résumé des produits dans le panier, le prix total et la possibilité de modifier la quantité d’un produit sélectionné ou bien de supprimer celui-ci.</t>
+  </si>
+  <si>
+    <t>Ouvrir la page panier et y retrouver les élément choisi par l'utilisateur. Il pourra églement y modifier la quantité ou supprimer un élément.</t>
+  </si>
+  <si>
+    <t>Affichage du panier avec tous les éléments commander</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sur la page panier remplir le formulaire avec des caratère valide pour chaque champ. Et envoi celui-ci au back-end </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affiche d'un message d'erreur si les caratère ne sont pas valide. Et si tout est bon l'envoi au back end avec une message pour etre sur de la confirmation. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ouvrir la page confirmation ou l'utilisateur retrouve sont numéro de commande </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affichage de la page confirmation et du numéro de commande </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="18.0"/>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Montserrat"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Montserrat"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="14"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Montserrat"/>
     </font>
   </fonts>
@@ -71,7 +126,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -81,7 +136,13 @@
     </fill>
   </fills>
   <borders count="17">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
@@ -95,8 +156,10 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -106,6 +169,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -120,6 +184,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -134,6 +199,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -142,17 +208,22 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -161,9 +232,11 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -172,9 +245,11 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -189,8 +264,10 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -200,6 +277,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -214,6 +292,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -228,6 +307,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -242,8 +322,10 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -253,6 +335,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -267,6 +350,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -281,92 +365,88 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -556,26 +636,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="7.29"/>
-    <col customWidth="1" min="2" max="3" width="58.43"/>
-    <col customWidth="1" min="4" max="4" width="57.86"/>
-    <col customWidth="1" min="5" max="5" width="52.71"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="3" width="58.44140625" customWidth="1"/>
+    <col min="4" max="4" width="57.88671875" customWidth="1"/>
+    <col min="5" max="5" width="52.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="31.5" customHeight="1">
+    <row r="1" spans="1:5" ht="31.5" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -590,9 +675,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="34.799999999999997">
       <c r="A2" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>4</v>
@@ -607,157 +692,190 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="104.4">
       <c r="A3" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="13">
-        <v>3.0</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="13">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="69.599999999999994">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="121.8">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="87">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17.399999999999999">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="17"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="17"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="17"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="17"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="17"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="17"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="17"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="16"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="17"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="17"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="16"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="17"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="17"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="16"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="17"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="16"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="17"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="16"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="17"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="16"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" spans="1:5" ht="17.399999999999999">
+      <c r="A8" s="14"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" spans="1:5" ht="17.399999999999999">
+      <c r="A9" s="14"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+    </row>
+    <row r="10" spans="1:5" ht="17.399999999999999">
+      <c r="A10" s="14"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:5" ht="17.399999999999999">
+      <c r="A11" s="14"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12" spans="1:5" ht="17.399999999999999">
+      <c r="A12" s="14"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="1:5" ht="17.399999999999999">
+      <c r="A13" s="14"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" spans="1:5" ht="17.399999999999999">
+      <c r="A14" s="14"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="1:5" ht="17.399999999999999">
+      <c r="A15" s="14"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" spans="1:5" ht="17.399999999999999">
+      <c r="A16" s="14"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="1:5" ht="17.399999999999999">
+      <c r="A17" s="14"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="13"/>
+    </row>
+    <row r="18" spans="1:5" ht="17.399999999999999">
+      <c r="A18" s="14"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="1:5" ht="17.399999999999999">
+      <c r="A19" s="14"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="13"/>
+    </row>
+    <row r="20" spans="1:5" ht="17.399999999999999">
+      <c r="A20" s="14"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="1:5" ht="17.399999999999999">
+      <c r="A21" s="14"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="1:5" ht="17.399999999999999">
+      <c r="A22" s="15"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="18"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>